<commit_message>
pre merge with obi
Former-commit-id: f34f034eb1fc0ee4474f32acb864135ba44244fb
</commit_message>
<xml_diff>
--- a/db/dummydata/gc_hubs.xlsx
+++ b/db/dummydata/gc_hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>STATUS</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>PHOTO</t>
+  </si>
+  <si>
+    <t>IMPORT_CHARGES</t>
+  </si>
+  <si>
+    <t>EXPORT_CHARGES</t>
+  </si>
+  <si>
+    <t>PRE_CARRIAGE</t>
+  </si>
+  <si>
+    <t>ON_CARRIAGE</t>
   </si>
   <si>
     <t>active</t>
@@ -143,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -156,6 +168,10 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font>
+      <b/>
+      <name val="Arial"/>
     </font>
     <font/>
     <font>
@@ -205,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -218,35 +234,38 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -311,394 +330,402 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6">
         <v>57.694253</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>11.854048</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>14</v>
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="7">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8">
         <v>30.626539</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>122.064958</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8">
         <v>57.668079</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>12.291456</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>14</v>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>31.141906</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>121.813579</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="10">
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="11">
         <v>59.650856</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="11">
         <v>17.931097</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
+      <c r="G6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="12">
         <v>55.535558</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="12">
         <v>13.363027</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
+      <c r="G7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="12">
         <v>22.316265</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="14">
         <v>113.939724</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="14"/>
+      <c r="G8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11">
         <v>29.826602</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="14">
         <v>121.462084</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>33</v>
+      <c r="G9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11">
         <v>38.96542</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="14">
         <v>121.539683</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="14"/>
+      <c r="G10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10">
+      <c r="A11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11">
         <v>36.266199</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="14">
         <v>120.383413</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11">
         <v>22.634996</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="14">
         <v>113.812407</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="A13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10">
+      <c r="A13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11">
         <v>39.130656</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="14">
         <v>117.35817</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="9"/>
+      <c r="G13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="I14" s="9"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="9"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="I17" s="9"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" ht="12.0" customHeight="1"/>
     <row r="19" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
hub view 90 percent fone
Former-commit-id: f1ac2651bbf44f322f0c03cf6e3f4eb89dbc1141
</commit_message>
<xml_diff>
--- a/db/dummydata/gc_hubs.xlsx
+++ b/db/dummydata/gc_hubs.xlsx
@@ -64,7 +64,7 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t>Port 4, Indiska Oceanen 11, 418 34 Göteborg, Sverige</t>
+    <t>Indiska Oceanen 11, 418 34 Göteborg, Sverige</t>
   </si>
   <si>
     <t>https://assets.itsmycargo.com/assets/cityimages/Gothenburg_sm.jpg</t>
@@ -244,10 +244,10 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -366,18 +366,18 @@
         <v>15</v>
       </c>
       <c r="E2" s="6">
-        <v>57.694253</v>
+        <v>57.6945306</v>
       </c>
       <c r="F2" s="7">
-        <v>11.854048</v>
+        <v>11.851909</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -391,19 +391,19 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>30.626539</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>122.064958</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -417,7 +417,7 @@
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>57.668079</v>
       </c>
       <c r="F4" s="6">
@@ -429,7 +429,7 @@
       <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -455,7 +455,7 @@
       <c r="H5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>